<commit_message>
Tweaks following the build of the first few boards, this is mostly minor dimensional fixes here and there. Also fixed a bom issue, one of the parts came on a giant reel instead of tape.
</commit_message>
<xml_diff>
--- a/bom/SLS BOM.xlsx
+++ b/bom/SLS BOM.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,11 +12,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>part/description</t>
   </si>
   <si>
+    <t>A97581-ND</t>
+  </si>
+  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -37,148 +41,136 @@
     <t>5-1634503-1</t>
   </si>
   <si>
-    <t>A97581-ND</t>
+    <t>732-5647-1-ND</t>
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/5-1634503-1/A97581-ND/1755969</t>
   </si>
   <si>
+    <t>LT6003IS5#TRMPBFCT-ND</t>
+  </si>
+  <si>
+    <t>296-20735-1-ND</t>
+  </si>
+  <si>
+    <t>SMD030F-2018-2CT-ND</t>
+  </si>
+  <si>
+    <t>SMBJ15D-M3/HGIDKR-ND</t>
+  </si>
+  <si>
+    <t>1KSMB6.8ACT-ND</t>
+  </si>
+  <si>
+    <t>445-8818-1-ND</t>
+  </si>
+  <si>
     <t>Wurth Threaded M3 Insert</t>
   </si>
   <si>
     <t>7466003R</t>
   </si>
   <si>
-    <t>732-5647-1-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/wurth-electronics-inc/7466003R/732-5647-1-ND/4915484</t>
   </si>
   <si>
+    <t>445-7878-1-ND</t>
+  </si>
+  <si>
+    <t>DMP3056L-7DICT-ND</t>
+  </si>
+  <si>
     <t>xtra slow opamp LT6003</t>
   </si>
   <si>
     <t>LT6003IS5#TRMPBF</t>
   </si>
   <si>
-    <t>LT6003IS5#TRMPBFCT-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/linear-technology-analog-devices/LT6003IS5-TRMPBF/LT6003IS5-TRMPBFCT-ND/1964949</t>
   </si>
   <si>
-    <t>polyzen 16v input protection</t>
-  </si>
-  <si>
-    <t>ZEN164V130A24LS</t>
-  </si>
-  <si>
-    <t>ZEN164V130A24LSCT-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/littelfuse-inc/ZEN164V130A24LS/ZEN164V130A24LSCT-ND/1618691</t>
-  </si>
-  <si>
     <t>5V 7905 linear reg</t>
   </si>
   <si>
+    <t>ZXTN25100DFHCT-ND</t>
+  </si>
+  <si>
     <t>UA79M05CKVURG3</t>
   </si>
   <si>
-    <t>296-20735-1-ND</t>
+    <t>P165HCT-ND</t>
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/texas-instruments/UA79M05CKVURG3/296-20735-1-ND/1197757</t>
   </si>
   <si>
+    <t>P4.02KHCT-ND</t>
+  </si>
+  <si>
+    <t>P442HCT-ND</t>
+  </si>
+  <si>
     <t>800mA PTC</t>
   </si>
   <si>
     <t>SMD030F-2018-2</t>
   </si>
   <si>
-    <t>SMD030F-2018-2CT-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/littelfuse-inc/SMD030F-2018-2/SMD030F-2018-2CT-ND/3720149</t>
   </si>
   <si>
     <t>15v TVS</t>
   </si>
   <si>
-    <t>SMBJ15D-M3/HGIDKR-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/vishay-semiconductor-diodes-division/SMBJ15D-M3-H/SMBJ15D-M3-HGIDKR-ND/5253094</t>
+    <t>SMBJ15D-M3/HGICT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/vishay-semiconductor-diodes-division/SMBJ15D-M3-H/SMBJ15D-M3-HGICT-ND/5253063</t>
   </si>
   <si>
     <t>5.8v TVS</t>
   </si>
   <si>
-    <t>1KSMB6.8ACT-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/littelfuse-inc/1KSMB6.8A/1KSMB6.8ACT-ND/2699826</t>
   </si>
   <si>
     <t>.1uF 0603 cap</t>
   </si>
   <si>
-    <t>445-8818-1-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/tdk-corporation/C1608X8R1H104K080AB/445-8818-1-ND/3248223</t>
   </si>
   <si>
     <t>1uF 0603</t>
   </si>
   <si>
-    <t>445-7878-1-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/tdk-corporation/CGA3E3X5R1H105K080AB/445-7878-1-ND/2781382</t>
   </si>
   <si>
     <t>PFet</t>
   </si>
   <si>
-    <t>DMP3056L-7DICT-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/diodes-incorporated/DMP3056L-7/DMP3056L-7DICT-ND/5126873</t>
   </si>
   <si>
     <t>NPN</t>
   </si>
   <si>
-    <t>ZXTN25100DFHCT-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/diodes-incorporated/ZXTN25100DFHTA/ZXTN25100DFHCT-ND/1137308</t>
   </si>
   <si>
     <t>165ohm 0603 resistor</t>
   </si>
   <si>
-    <t>P165HCT-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en/resistors/chip-resistor-surface-mount/52?k=&amp;pkeyword=&amp;v=10&amp;FV=c0001%2C142c040c%2C1f140000%2Cmu165+Ohms%7C2085%2Cffe00034%2C1c0002&amp;quantity=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;pageSize=25</t>
   </si>
   <si>
     <t>4020ohm 0603 resistor</t>
   </si>
   <si>
-    <t>P4.02KHCT-ND</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en/resistors/chip-resistor-surface-mount/52?k=&amp;pkeyword=&amp;v=10&amp;FV=c0001%2C1c0002%2C142c040c%2C1f140000%2Cffe00034%2Cmu4.02+kOhms%7C2085&amp;quantity=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;pageSize=25</t>
   </si>
   <si>
     <t>442ohm 0603 resistor</t>
-  </si>
-  <si>
-    <t>P442HCT-ND</t>
   </si>
   <si>
     <t>https://www.digikey.com/products/en/resistors/chip-resistor-surface-mount/52?k=&amp;pkeyword=&amp;pv2085=u442+Ohms&amp;FV=c0001%2C1c0002%2C142c040c%2C1f140000%2Cffe00034%2Cfffc000a&amp;quantity=0&amp;ColumnSort=0&amp;page=1&amp;stock=1&amp;pageSize=25</t>
@@ -188,7 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -199,6 +191,11 @@
     </font>
     <font>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -229,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -239,11 +236,14 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -251,7 +251,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -263,6 +269,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -289,301 +299,281 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
         <v>3.0</v>
       </c>
-      <c r="C2" s="3">
-        <v>9.0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4">
         <v>4.0</v>
       </c>
-      <c r="C3" s="3">
-        <v>16.0</v>
+      <c r="C3" s="5">
+        <v>20.0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4">
         <v>1.0</v>
       </c>
-      <c r="C4" s="3">
-        <v>3.0</v>
+      <c r="C4" s="5">
+        <v>5.0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="3">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4">
         <v>1.0</v>
       </c>
-      <c r="C5" s="3">
-        <v>3.0</v>
+      <c r="C5" s="4">
+        <v>5.0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>21</v>
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="3">
+        <v>32</v>
+      </c>
+      <c r="B6" s="4">
         <v>1.0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>5.0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="3">
+        <v>35</v>
+      </c>
+      <c r="B7" s="4">
         <v>1.0</v>
       </c>
-      <c r="C7" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>29</v>
+      <c r="C7" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C8" s="6">
-        <v>3.0</v>
+        <v>38</v>
+      </c>
+      <c r="B8" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>10.0</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>32</v>
+        <v>15</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="3">
+        <v>40</v>
+      </c>
+      <c r="B9" s="4">
         <v>2.0</v>
       </c>
-      <c r="C9" s="6">
-        <v>6.0</v>
+      <c r="C9" s="7">
+        <v>10.0</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C10" s="6">
+        <v>42</v>
+      </c>
+      <c r="B10" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C10" s="7">
         <v>10.0</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>38</v>
+        <v>20</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="3">
-        <v>3.0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>10.0</v>
+        <v>44</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>5.0</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="3">
+        <v>46</v>
+      </c>
+      <c r="B12" s="4">
         <v>1.0</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>5.0</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>44</v>
+        <v>26</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="3">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4">
         <v>1.0</v>
       </c>
-      <c r="C13" s="6">
-        <v>5.0</v>
+      <c r="C13" s="7">
+        <v>10.0</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C14" s="6">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="7">
         <v>10.0</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>50</v>
+        <v>30</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C15" s="6">
+        <v>52</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="C15" s="7">
         <v>10.0</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C16" s="6">
-        <v>10.0</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -602,8 +592,137 @@
     <hyperlink r:id="rId12" ref="F13"/>
     <hyperlink r:id="rId13" ref="F14"/>
     <hyperlink r:id="rId14" ref="F15"/>
-    <hyperlink r:id="rId15" ref="F16"/>
   </hyperlinks>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId15"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="28.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="7">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="7">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="7">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="7">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="7">
+        <v>10.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>